<commit_message>
brute force push through on part 2 of day 3
</commit_message>
<xml_diff>
--- a/src/main/groovy/com/jabeg/excel_helpers/day3.xlsx
+++ b/src/main/groovy/com/jabeg/excel_helpers/day3.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\IdeaProjects\AdventDay1\src\main\groovy\com\jabeg\excel_helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{AA50F285-9306-41A8-BA31-68186B65B52E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{AA50F285-9306-41A8-BA31-68186B65B52E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Part 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Loop Counter</t>
   </si>
@@ -45,6 +46,15 @@
   </si>
   <si>
     <t>Lastly subtract the value of the loop counter from the value you found in the previous step. Make sure to account for center(1)</t>
+  </si>
+  <si>
+    <t>Brute force this shit</t>
+  </si>
+  <si>
+    <t>Heres the answer</t>
+  </si>
+  <si>
+    <t>Provided</t>
   </si>
 </sst>
 </file>
@@ -74,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,8 +121,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,11 +145,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -146,12 +177,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EF722E-9E12-4A80-8BFB-10434DF0BDA1}">
   <dimension ref="A1:R717"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,7 +1122,7 @@
       <c r="P13" s="2">
         <v>169</v>
       </c>
-      <c r="R13" s="11" t="s">
+      <c r="R13" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1095,7 +1138,7 @@
         <f t="shared" si="1"/>
         <v>218</v>
       </c>
-      <c r="R14" s="11"/>
+      <c r="R14" s="10"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1109,7 +1152,7 @@
         <f t="shared" si="1"/>
         <v>281</v>
       </c>
-      <c r="R15" s="11"/>
+      <c r="R15" s="10"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1123,7 +1166,7 @@
         <f t="shared" si="1"/>
         <v>352</v>
       </c>
-      <c r="R16" s="11"/>
+      <c r="R16" s="10"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -1137,7 +1180,7 @@
         <f t="shared" si="1"/>
         <v>431</v>
       </c>
-      <c r="R17" s="11"/>
+      <c r="R17" s="10"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -1151,7 +1194,7 @@
         <f t="shared" si="1"/>
         <v>518</v>
       </c>
-      <c r="R18" s="10" t="s">
+      <c r="R18" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1167,7 +1210,7 @@
         <f t="shared" si="1"/>
         <v>613</v>
       </c>
-      <c r="R19" s="10"/>
+      <c r="R19" s="11"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
@@ -1181,7 +1224,7 @@
         <f t="shared" si="1"/>
         <v>716</v>
       </c>
-      <c r="R20" s="10"/>
+      <c r="R20" s="11"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
@@ -1195,7 +1238,7 @@
         <f t="shared" si="1"/>
         <v>827</v>
       </c>
-      <c r="R21" s="10"/>
+      <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
@@ -1209,7 +1252,7 @@
         <f t="shared" si="1"/>
         <v>946</v>
       </c>
-      <c r="R22" s="10"/>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
@@ -1223,7 +1266,7 @@
         <f t="shared" si="1"/>
         <v>1073</v>
       </c>
-      <c r="R23" s="10"/>
+      <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
@@ -5380,4 +5423,294 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D105535E-BA4E-4CE7-91A7-057321B19AB6}">
+  <dimension ref="C3:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="10" width="8.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C3" s="16">
+        <f>D3+D4+C4</f>
+        <v>363010</v>
+      </c>
+      <c r="D3" s="17">
+        <f>E3+E4+D4+C4</f>
+        <v>349975</v>
+      </c>
+      <c r="E3" s="17">
+        <f>F3+F4+E4+D4</f>
+        <v>330785</v>
+      </c>
+      <c r="F3" s="17">
+        <f>G3+G4+F4+E4</f>
+        <v>312453</v>
+      </c>
+      <c r="G3" s="17">
+        <f>H3+H4+G4+F4</f>
+        <v>295229</v>
+      </c>
+      <c r="H3" s="17">
+        <f>I3+I4+H4+G4</f>
+        <v>279138</v>
+      </c>
+      <c r="I3" s="17">
+        <f>J3+J4+I4+H4</f>
+        <v>266330</v>
+      </c>
+      <c r="J3" s="17">
+        <f>J4+I4</f>
+        <v>130654</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="17">
+        <f>D4+D5</f>
+        <v>6591</v>
+      </c>
+      <c r="D4" s="17">
+        <f>E4+E5+D5</f>
+        <v>6444</v>
+      </c>
+      <c r="E4" s="17">
+        <f>F4+F5+E5+D5</f>
+        <v>6155</v>
+      </c>
+      <c r="F4" s="17">
+        <f>G4+G5+F5+E5</f>
+        <v>5733</v>
+      </c>
+      <c r="G4" s="17">
+        <f>H4+H5+G5+F5</f>
+        <v>5336</v>
+      </c>
+      <c r="H4" s="17">
+        <f>I4+I5+H5+G5</f>
+        <v>5022</v>
+      </c>
+      <c r="I4" s="17">
+        <f>I5+H5</f>
+        <v>2450</v>
+      </c>
+      <c r="J4" s="17">
+        <f>J5+I5+I4</f>
+        <v>128204</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="17">
+        <f>C4+D4+D5+D6</f>
+        <v>13486</v>
+      </c>
+      <c r="D5" s="12">
+        <v>147</v>
+      </c>
+      <c r="E5" s="12">
+        <v>142</v>
+      </c>
+      <c r="F5" s="12">
+        <v>133</v>
+      </c>
+      <c r="G5" s="12">
+        <v>122</v>
+      </c>
+      <c r="H5" s="12">
+        <v>59</v>
+      </c>
+      <c r="I5" s="17">
+        <f>I6+H6+H5</f>
+        <v>2391</v>
+      </c>
+      <c r="J5" s="17">
+        <f>J6+I6+I5+I4</f>
+        <v>123363</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6" s="17">
+        <f>D6+D5+C5+D7</f>
+        <v>14267</v>
+      </c>
+      <c r="D6" s="12">
+        <v>304</v>
+      </c>
+      <c r="E6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12">
+        <v>4</v>
+      </c>
+      <c r="G6" s="12">
+        <v>2</v>
+      </c>
+      <c r="H6" s="12">
+        <v>57</v>
+      </c>
+      <c r="I6" s="17">
+        <f>I7+H7+H6+H5</f>
+        <v>2275</v>
+      </c>
+      <c r="J6" s="17">
+        <f>J7+I7+I6+I5</f>
+        <v>116247</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C7" s="17">
+        <f>D7+D6+C6+D8</f>
+        <v>15252</v>
+      </c>
+      <c r="D7" s="12">
+        <v>330</v>
+      </c>
+      <c r="E7" s="12">
+        <v>10</v>
+      </c>
+      <c r="F7" s="12">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>54</v>
+      </c>
+      <c r="I7" s="17">
+        <f>I8+H8+H7+H6</f>
+        <v>2105</v>
+      </c>
+      <c r="J7" s="17">
+        <f>J8+I8+I7+I6</f>
+        <v>109476</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C8" s="17">
+        <f>D8+D7+C7+D9</f>
+        <v>16295</v>
+      </c>
+      <c r="D8" s="12">
+        <v>351</v>
+      </c>
+      <c r="E8" s="12">
+        <v>11</v>
+      </c>
+      <c r="F8" s="12">
+        <v>23</v>
+      </c>
+      <c r="G8" s="12">
+        <v>25</v>
+      </c>
+      <c r="H8" s="12">
+        <v>26</v>
+      </c>
+      <c r="I8" s="17">
+        <f>I9+H9+H8+H7</f>
+        <v>1968</v>
+      </c>
+      <c r="J8" s="17">
+        <f>J9+I9+I8+I7</f>
+        <v>103128</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="17">
+        <f>D9+D8+C8</f>
+        <v>17008</v>
+      </c>
+      <c r="D9" s="12">
+        <v>362</v>
+      </c>
+      <c r="E9" s="12">
+        <v>747</v>
+      </c>
+      <c r="F9" s="12">
+        <v>806</v>
+      </c>
+      <c r="G9" s="17">
+        <f>F9+F8+G8+H8</f>
+        <v>880</v>
+      </c>
+      <c r="H9" s="17">
+        <f>G9+G8+H8</f>
+        <v>931</v>
+      </c>
+      <c r="I9" s="17">
+        <f>H9+H8</f>
+        <v>957</v>
+      </c>
+      <c r="J9" s="17">
+        <f>J10+I10+I9+I8</f>
+        <v>98098</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="17">
+        <f>C9+D9</f>
+        <v>17370</v>
+      </c>
+      <c r="D10" s="17">
+        <f>C10+C9+D9+E9</f>
+        <v>35487</v>
+      </c>
+      <c r="E10" s="17">
+        <f>D10+D9+E9+F9</f>
+        <v>37402</v>
+      </c>
+      <c r="F10" s="17">
+        <f>E10+E9+F9+G9</f>
+        <v>39835</v>
+      </c>
+      <c r="G10" s="17">
+        <f>F10+F9+G9+H9</f>
+        <v>42452</v>
+      </c>
+      <c r="H10" s="17">
+        <f>G10+G9+H9+I9</f>
+        <v>45220</v>
+      </c>
+      <c r="I10" s="17">
+        <f>H10+H9+I9</f>
+        <v>47108</v>
+      </c>
+      <c r="J10" s="17">
+        <f>I10+I9</f>
+        <v>48065</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="14"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G13:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>